<commit_message>
5 Ekim Dersi Ödevi
</commit_message>
<xml_diff>
--- a/Ödevler/javahw3/hw6/MusteriYonetimiTablo.xlsx
+++ b/Ödevler/javahw3/hw6/MusteriYonetimiTablo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\JavaCamp2022\Ödevler\javahw3\hw6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2E130B-438A-430E-83E3-79BC602204DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E7CF89-B6BF-42B8-8F46-4F623B3B3F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="1704" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,16 +357,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1906</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>605792</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>137162</xdr:rowOff>
+      <xdr:rowOff>106681</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -381,12 +381,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6179820" y="1546860"/>
-          <a:ext cx="3539492" cy="1066802"/>
+          <a:off x="6196966" y="1266826"/>
+          <a:ext cx="3549014" cy="1316355"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 70248"/>
+            <a:gd name="adj1" fmla="val 73164"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>

</xml_diff>